<commit_message>
Alteração do Power Bi, arquivo em excel para economizar espaço e Notebook
</commit_message>
<xml_diff>
--- a/excel/agencias.xlsx
+++ b/excel/agencias.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +446,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>endereco</t>
+          <t>uf</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>cidade</t>
+          <t>data_abertura</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>uf</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>data_abertura</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>tipo_agencia</t>
         </is>
@@ -481,25 +471,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Av. Paulista, 1436 - Cerqueira César, São Paulo - SP, 01310-916</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>01/08/2015</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>01/08/2015</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
         <is>
           <t>Digital</t>
         </is>
@@ -516,25 +496,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Av. Paulista, 1436 - Cerqueira César, São Paulo - SP, 01310-916</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>01/01/2010</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>01/01/2010</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
         <is>
           <t>Física</t>
         </is>
@@ -551,25 +521,15 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Praça Sílvio Romero, 158 - Tatuapé, São Paulo - SP, 03323-000</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>14/06/2010</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>14/06/2010</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
         <is>
           <t>Física</t>
         </is>
@@ -586,25 +546,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Av. Francisco Glicério, 895 - Vila Lidia, Campinas - SP, 13012-000</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Campinas</t>
+          <t>04/03/2012</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>04/03/2012</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
         <is>
           <t>Física</t>
         </is>
@@ -621,25 +571,15 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Av. Antônio Carlos Costa, 1000 - Bela Vista, Osasco - SP, 06053-014</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Osasco</t>
+          <t>06/11/2013</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>06/11/2013</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
         <is>
           <t>Física</t>
         </is>
@@ -656,25 +596,15 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Av. Bento Gonçalves, 1924 - Partenon, Porto Alegre - RS, 90650-000</t>
+          <t>RS</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>01/12/2013</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
-        <is>
-          <t>RS</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>01/12/2013</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
         <is>
           <t>Física</t>
         </is>
@@ -691,25 +621,15 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R. Sen. Dantas, 15 - Centro, Rio de Janeiro - RJ, 20031-202</t>
+          <t>RJ</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>01/04/2015</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
-        <is>
-          <t>RJ</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>01/04/2015</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
         <is>
           <t>Física</t>
         </is>
@@ -726,25 +646,15 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Av. Brg. Faria Lima, 2491 - Jardim Paulistano, São Paulo - SP, 01452-000</t>
+          <t>SP</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>09/01/2018</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
-        <is>
-          <t>SP</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>09/01/2018</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
         <is>
           <t>Física</t>
         </is>
@@ -761,25 +671,15 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Av. Jorn. Rubéns de Arruda Ramos, 1280 - Centro, Florianópolis - SC, 88015-700</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Florianópolis</t>
+          <t>09/10/2019</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
-        <is>
-          <t>SC</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>09/10/2019</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
         <is>
           <t>Física</t>
         </is>
@@ -796,25 +696,15 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Av. Conselheiro Aguiar, 4432 - Boa Viagem, Recife - PE, 51021-020</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>09/10/2021</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
-        <is>
-          <t>PE</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>09/10/2021</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
         <is>
           <t>Física</t>
         </is>

</xml_diff>